<commit_message>
Commit testing files (I don`t know why it suggests commiting 112 files in total).
</commit_message>
<xml_diff>
--- a/MemoryGame/Testing Documentation/testing_android.xlsx
+++ b/MemoryGame/Testing Documentation/testing_android.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19635" windowHeight="9480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Android Version</t>
   </si>
@@ -94,13 +95,49 @@
   </si>
   <si>
     <t>Issue 12</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Black Text on Black Background - need a few different themes</t>
+  </si>
+  <si>
+    <t>General Problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -  </t>
+  </si>
+  <si>
+    <t>Game button positioning</t>
+  </si>
+  <si>
+    <t>Blank Activities</t>
+  </si>
+  <si>
+    <t>Sound off Button State</t>
+  </si>
+  <si>
+    <t>Nexus 7" Tab</t>
+  </si>
+  <si>
+    <t>4.8" Samsung S3</t>
+  </si>
+  <si>
+    <t>4.0" S3 Mini</t>
+  </si>
+  <si>
+    <t>10.1" Tab 2</t>
+  </si>
+  <si>
+    <t>Runs same as others, buttons tiny in top left corner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,16 +145,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,14 +176,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,324 +507,527 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q39"/>
+  <dimension ref="B2:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>8</v>
       </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>9</v>
       </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="2">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="2">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>10</v>
       </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>10</v>
       </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>11</v>
       </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>12</v>
       </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
+      <c r="B11" s="4">
         <v>3.2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>13</v>
       </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>14</v>
       </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="2:17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="2:17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="2:17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="2:17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C15">
+      <c r="C17" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="2:17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
         <v>4.3</v>
       </c>
-      <c r="C16">
+      <c r="C18" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
+      <c r="D18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="2:17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C17">
+      <c r="C19" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D20" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>3</v>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="2:17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K20" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P20" s="1">
-        <v>4.3</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-    </row>
+        <v>31</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:17" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>